<commit_message>
Projeto Venda Direta Finalizado
</commit_message>
<xml_diff>
--- a/Dropbox/PROJETO INTEGRADOR/DOCUMENTAÇÃO/Cronograma.xlsx
+++ b/Dropbox/PROJETO INTEGRADOR/DOCUMENTAÇÃO/Cronograma.xlsx
@@ -118,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +176,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -191,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -291,21 +298,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -313,7 +305,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -324,7 +316,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -337,22 +329,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -385,12 +362,6 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,15 +371,6 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -417,6 +379,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -720,7 +691,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -731,7 +702,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,17 +714,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -768,7 +739,7 @@
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -810,7 +781,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -831,7 +802,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -873,7 +844,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -894,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -915,7 +886,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -936,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -977,7 +948,7 @@
       <c r="E12" s="4">
         <v>1</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="11">
         <v>1</v>
       </c>
     </row>
@@ -999,7 +970,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -1020,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -1041,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -1059,33 +1030,35 @@
         <v>42466</v>
       </c>
       <c r="E16" s="4">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F16" s="8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="10">
+      <c r="C17" s="17"/>
+      <c r="D17" s="15">
+        <f>D16+E16+1</f>
+        <v>42513</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19">
         <f>AVERAGE(F3:F16)</f>
-        <v>0.87142857142857122</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="B3:E16">
     <sortCondition ref="D3:D16" customList="jan,fev,mar,abr,mai,jun,jul,ago,set,out,nov,dez"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="B17:E17"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F17">

</xml_diff>